<commit_message>
saving project state before coding new algo to match same view to uncovered nodes
</commit_message>
<xml_diff>
--- a/graph_expr/output/goodcol_outputs/am_lb3_1query__ansgrBYVIEWS_newcols.xlsx
+++ b/graph_expr/output/goodcol_outputs/am_lb3_1query__ansgrBYVIEWS_newcols.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t xml:space="preserve">*****************************************************</t>
   </si>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">1019.00 MB</t>
   </si>
   <si>
-    <t xml:space="preserve"># of edges</t>
+    <t xml:space="preserve"># of edges in SG</t>
   </si>
   <si>
     <t xml:space="preserve">WITH VIEWS, angr</t>
@@ -170,23 +170,36 @@
     <t xml:space="preserve">no views, angr, NO FILTER, alltimes</t>
   </si>
   <si>
-    <t xml:space="preserve">no views, simgr, only prefilter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no views, simgr, NO FILTER</t>
+    <t xml:space="preserve">no views, summ graph, only prefilter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no views, match graph, NO FILTER</t>
   </si>
   <si>
     <t xml:space="preserve">alltimes: includes time it takes to compute occurrence lists to be used as input to create answer graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check if query is too general bc may take too much time. Desc edges take long time to compute, so stop at 10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulation graph must uses simulation filtering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also try using prefilter + simulation to produce even smaller graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maybe ‘with views’ enumTime is faster b/c the paths Mijoin uses to find answers is more efficient???</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -239,7 +252,28 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -300,7 +334,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,7 +367,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,7 +375,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -349,15 +387,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -370,6 +424,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -380,8 +494,8 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A16 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.01953125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -729,10 +843,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:IV16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.01171875" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -742,7 +856,8 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="2" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="12.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="2" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="2" width="10"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,37 +943,37 @@
         <v>45</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="10" t="n">
         <v>1.54</v>
       </c>
-      <c r="D3" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9" t="n">
+      <c r="D3" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="n">
         <v>0.33</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="10" t="n">
         <v>0.13</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="11" t="n">
         <v>2.01</v>
       </c>
-      <c r="H3" s="9" t="n">
+      <c r="H3" s="10" t="n">
         <v>403394</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="10" t="n">
         <v>163085</v>
       </c>
-      <c r="J3" s="9" t="n">
+      <c r="J3" s="10" t="n">
         <v>149987</v>
       </c>
-      <c r="K3" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="9" t="n">
+      <c r="K3" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="10" t="n">
         <v>336526</v>
       </c>
-      <c r="M3" s="9" t="n">
+      <c r="M3" s="10" t="n">
         <f aca="false">L3-J3</f>
         <v>186539</v>
       </c>
@@ -868,38 +983,38 @@
       <c r="A4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11" t="n">
+      <c r="B4" s="12"/>
+      <c r="C4" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13" t="n">
         <v>0.34</v>
       </c>
-      <c r="F4" s="11" t="n">
+      <c r="F4" s="13" t="n">
         <v>0.17</v>
       </c>
-      <c r="G4" s="12" t="n">
+      <c r="G4" s="14" t="n">
         <v>0.51</v>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="H4" s="13" t="n">
         <v>403394</v>
       </c>
-      <c r="I4" s="11" t="n">
+      <c r="I4" s="13" t="n">
         <v>163085</v>
       </c>
-      <c r="J4" s="11" t="n">
+      <c r="J4" s="13" t="n">
         <v>149987</v>
       </c>
-      <c r="K4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="11" t="n">
+      <c r="K4" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13" t="n">
         <v>336526</v>
       </c>
-      <c r="M4" s="9" t="n">
+      <c r="M4" s="10" t="n">
         <f aca="false">L4-J4</f>
         <v>186539</v>
       </c>
@@ -1148,88 +1263,88 @@
       <c r="IV4" s="3"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="16" t="n">
         <v>1.64</v>
       </c>
-      <c r="D5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="n">
+      <c r="D5" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16" t="n">
         <v>0.81</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="16" t="n">
         <v>0.13</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="17" t="n">
         <v>2.59</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="16" t="n">
         <v>403394</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="16" t="n">
         <v>163085</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="16" t="n">
         <v>149987</v>
       </c>
-      <c r="K5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5" t="n">
+      <c r="K5" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="16" t="n">
         <v>336526</v>
       </c>
-      <c r="M5" s="2" t="n">
+      <c r="M5" s="18" t="n">
         <f aca="false">L5-J5</f>
         <v>186539</v>
       </c>
       <c r="N5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="n">
+      <c r="C6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16" t="n">
         <v>1.33</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="16" t="n">
         <v>0.15</v>
       </c>
-      <c r="G6" s="13" t="n">
+      <c r="G6" s="17" t="n">
         <v>1.48</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="16" t="n">
         <v>403394</v>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="16" t="n">
         <v>163085</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="16" t="n">
         <v>149987</v>
       </c>
-      <c r="K6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5" t="n">
+      <c r="K6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16" t="n">
         <v>336526</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="M6" s="18" t="n">
         <f aca="false">L6-J6</f>
         <v>186539</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="3" t="n">
@@ -1244,7 +1359,7 @@
       <c r="F7" s="3" t="n">
         <v>0.21</v>
       </c>
-      <c r="G7" s="14" t="n">
+      <c r="G7" s="19" t="n">
         <v>1.61</v>
       </c>
       <c r="H7" s="3" t="n">
@@ -1284,7 +1399,7 @@
       <c r="F8" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="G8" s="14" t="n">
+      <c r="G8" s="19" t="n">
         <v>0.94</v>
       </c>
       <c r="H8" s="3" t="n">
@@ -1339,6 +1454,29 @@
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
     </row>
+    <row r="11" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>